<commit_message>
add graph horizontal scaling
</commit_message>
<xml_diff>
--- a/finmail/output.xlsx
+++ b/finmail/output.xlsx
@@ -546,31 +546,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>454.93</v>
+        <v>454.61</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="D2">
-        <v>0.37</v>
+        <v>-0.09</v>
       </c>
       <c r="E2">
-        <v>10.77</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="F2">
-        <v>1.23</v>
+        <v>1.3</v>
       </c>
       <c r="G2">
-        <v>8.630000000000001</v>
+        <v>7.01</v>
       </c>
       <c r="H2">
-        <v>20.28</v>
+        <v>20.19</v>
       </c>
       <c r="I2">
-        <v>16.72</v>
+        <v>16.84</v>
       </c>
       <c r="J2">
-        <v>80.5</v>
+        <v>79.28</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -578,31 +578,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>14281.76</v>
+        <v>14258.49</v>
       </c>
       <c r="C3">
-        <v>0.29</v>
+        <v>-0.16</v>
       </c>
       <c r="D3">
-        <v>0.58</v>
+        <v>-0.05</v>
       </c>
       <c r="E3">
-        <v>12.96</v>
+        <v>11.49</v>
       </c>
       <c r="F3">
-        <v>1.87</v>
+        <v>1.59</v>
       </c>
       <c r="G3">
-        <v>9.01</v>
+        <v>7.69</v>
       </c>
       <c r="H3">
-        <v>36.45</v>
+        <v>36.23</v>
       </c>
       <c r="I3">
-        <v>29.25</v>
+        <v>29.81</v>
       </c>
       <c r="J3">
-        <v>96.36</v>
+        <v>94.51000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -610,31 +610,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>35416.98</v>
+        <v>35430.42</v>
       </c>
       <c r="C4">
-        <v>0.24</v>
+        <v>0.04</v>
       </c>
       <c r="D4">
-        <v>0.9399999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="E4">
-        <v>9.25</v>
+        <v>7.6</v>
       </c>
       <c r="F4">
-        <v>1.51</v>
+        <v>2.04</v>
       </c>
       <c r="G4">
-        <v>7.12</v>
+        <v>4.94</v>
       </c>
       <c r="H4">
-        <v>6.85</v>
+        <v>6.89</v>
       </c>
       <c r="I4">
-        <v>4.63</v>
+        <v>4.66</v>
       </c>
       <c r="J4">
-        <v>39.77</v>
+        <v>38.73</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -642,31 +642,31 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>12.69</v>
+        <v>12.98</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2.29</v>
       </c>
       <c r="D5">
-        <v>-4.94</v>
+        <v>1.01</v>
       </c>
       <c r="E5">
-        <v>-40.34</v>
+        <v>-34.28</v>
       </c>
       <c r="F5">
-        <v>-8.57</v>
+        <v>-4.35</v>
       </c>
       <c r="G5">
-        <v>-18.91</v>
+        <v>-11.1</v>
       </c>
       <c r="H5">
-        <v>-41.44</v>
+        <v>-40.1</v>
       </c>
       <c r="I5">
-        <v>-42.86</v>
+        <v>-40.7</v>
       </c>
       <c r="J5">
-        <v>-32.46</v>
+        <v>-28.17</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -674,31 +674,31 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>5.26</v>
+        <v>5.24</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-0.38</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>-0.38</v>
       </c>
       <c r="E6">
-        <v>-0.75</v>
+        <v>-1.32</v>
       </c>
       <c r="F6">
         <v>-1.13</v>
       </c>
       <c r="G6">
-        <v>1.15</v>
+        <v>0.38</v>
       </c>
       <c r="H6">
-        <v>23.47</v>
+        <v>23</v>
       </c>
       <c r="I6">
-        <v>25.84</v>
+        <v>23.29</v>
       </c>
       <c r="J6">
-        <v>127.71</v>
+        <v>126.84</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -706,31 +706,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>4.29</v>
+        <v>4.22</v>
       </c>
       <c r="C7">
-        <v>-2.72</v>
+        <v>-1.63</v>
       </c>
       <c r="D7">
-        <v>-2.94</v>
+        <v>-4.95</v>
       </c>
       <c r="E7">
-        <v>-10.06</v>
+        <v>-12.08</v>
       </c>
       <c r="F7">
-        <v>0.47</v>
+        <v>-0.47</v>
       </c>
       <c r="G7">
-        <v>15.95</v>
+        <v>9.9</v>
       </c>
       <c r="H7">
-        <v>7.25</v>
+        <v>5.5</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>7.65</v>
       </c>
       <c r="J7">
-        <v>50</v>
+        <v>48.07</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -738,31 +738,31 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>4.34</v>
+        <v>4.27</v>
       </c>
       <c r="C8">
-        <v>-1.14</v>
+        <v>-1.61</v>
       </c>
       <c r="D8">
-        <v>-1.81</v>
+        <v>-3.39</v>
       </c>
       <c r="E8">
-        <v>-10.33</v>
+        <v>-12.5</v>
       </c>
       <c r="F8">
-        <v>5.34</v>
+        <v>4.4</v>
       </c>
       <c r="G8">
-        <v>20.22</v>
+        <v>15.72</v>
       </c>
       <c r="H8">
-        <v>11.86</v>
+        <v>10.05</v>
       </c>
       <c r="I8">
-        <v>17.3</v>
+        <v>13.87</v>
       </c>
       <c r="J8">
-        <v>42.76</v>
+        <v>41.86</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -770,31 +770,31 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>4.52</v>
+        <v>4.45</v>
       </c>
       <c r="C9">
-        <v>-0.22</v>
+        <v>-1.55</v>
       </c>
       <c r="D9">
-        <v>-1.31</v>
+        <v>-2.2</v>
       </c>
       <c r="E9">
-        <v>-9.960000000000001</v>
+        <v>-11.53</v>
       </c>
       <c r="F9">
-        <v>6.86</v>
+        <v>5.95</v>
       </c>
       <c r="G9">
-        <v>18.02</v>
+        <v>14.69</v>
       </c>
       <c r="H9">
-        <v>13.85</v>
+        <v>12.09</v>
       </c>
       <c r="I9">
-        <v>20.53</v>
+        <v>17.11</v>
       </c>
       <c r="J9">
-        <v>35.74</v>
+        <v>34.44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -805,28 +805,28 @@
         <v>4.48</v>
       </c>
       <c r="C10">
-        <v>2.52</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>-1.54</v>
+        <v>-0.44</v>
       </c>
       <c r="E10">
-        <v>2.28</v>
+        <v>3.46</v>
       </c>
       <c r="F10">
-        <v>-9.68</v>
+        <v>-9.859999999999999</v>
       </c>
       <c r="G10">
-        <v>1.59</v>
+        <v>-5.88</v>
       </c>
       <c r="H10">
         <v>-11.46</v>
       </c>
       <c r="I10">
-        <v>-15.95</v>
+        <v>-17.95</v>
       </c>
       <c r="J10">
-        <v>-10.58</v>
+        <v>-10.4</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -834,31 +834,31 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>120.07</v>
+        <v>120.46</v>
       </c>
       <c r="C11">
-        <v>-1.36</v>
+        <v>0.32</v>
       </c>
       <c r="D11">
-        <v>0.82</v>
+        <v>-1.54</v>
       </c>
       <c r="E11">
-        <v>8.550000000000001</v>
+        <v>6.32</v>
       </c>
       <c r="F11">
-        <v>0.92</v>
+        <v>3.06</v>
       </c>
       <c r="G11">
-        <v>2.69</v>
+        <v>2.44</v>
       </c>
       <c r="H11">
-        <v>1.42</v>
+        <v>1.75</v>
       </c>
       <c r="I11">
-        <v>0.41</v>
+        <v>0.79</v>
       </c>
       <c r="J11">
-        <v>112.89</v>
+        <v>113.73</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -866,31 +866,31 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>90.63</v>
+        <v>92.27</v>
       </c>
       <c r="C12">
-        <v>0.13</v>
+        <v>1.81</v>
       </c>
       <c r="D12">
-        <v>3.04</v>
+        <v>2.29</v>
       </c>
       <c r="E12">
-        <v>13.36</v>
+        <v>15.68</v>
       </c>
       <c r="F12">
-        <v>7.03</v>
+        <v>6.17</v>
       </c>
       <c r="G12">
-        <v>34.67</v>
+        <v>33.76</v>
       </c>
       <c r="H12">
-        <v>45.33</v>
+        <v>47.96</v>
       </c>
       <c r="I12">
-        <v>42.61</v>
+        <v>43.34</v>
       </c>
       <c r="J12">
-        <v>285.33</v>
+        <v>297.89</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -898,31 +898,31 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>409.01</v>
+        <v>409.82</v>
       </c>
       <c r="C13">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="D13">
-        <v>0.01</v>
+        <v>-0.12</v>
       </c>
       <c r="E13">
-        <v>12.34</v>
+        <v>10.04</v>
       </c>
       <c r="F13">
-        <v>-1.04</v>
+        <v>-0.54</v>
       </c>
       <c r="G13">
-        <v>10.6</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="H13">
-        <v>18.34</v>
+        <v>18.58</v>
       </c>
       <c r="I13">
-        <v>19.42</v>
+        <v>20.16</v>
       </c>
       <c r="J13">
-        <v>113.83</v>
+        <v>109.55</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -930,31 +930,31 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>190.4</v>
+        <v>189.37</v>
       </c>
       <c r="C14">
-        <v>0.32</v>
+        <v>-0.54</v>
       </c>
       <c r="D14">
-        <v>-0.13</v>
+        <v>-1.01</v>
       </c>
       <c r="E14">
-        <v>13.33</v>
+        <v>11.35</v>
       </c>
       <c r="F14">
-        <v>1.6</v>
+        <v>0.93</v>
       </c>
       <c r="G14">
-        <v>6.01</v>
+        <v>4.93</v>
       </c>
       <c r="H14">
-        <v>47.36</v>
+        <v>46.56</v>
       </c>
       <c r="I14">
-        <v>32.76</v>
+        <v>34.89</v>
       </c>
       <c r="J14">
-        <v>341.97</v>
+        <v>341.94</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -962,31 +962,31 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>136.38</v>
+        <v>137.31</v>
       </c>
       <c r="C15">
-        <v>-0.4</v>
+        <v>0.68</v>
       </c>
       <c r="D15">
-        <v>0.38</v>
+        <v>1.02</v>
       </c>
       <c r="E15">
-        <v>11.37</v>
+        <v>13.35</v>
       </c>
       <c r="F15">
-        <v>13.29</v>
+        <v>14.61</v>
       </c>
       <c r="G15">
-        <v>7.12</v>
+        <v>7.87</v>
       </c>
       <c r="H15">
-        <v>12.31</v>
+        <v>13.08</v>
       </c>
       <c r="I15">
-        <v>7.07</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="J15">
-        <v>60.75</v>
+        <v>66.31999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -994,31 +994,31 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>48.84</v>
+        <v>49.57</v>
       </c>
       <c r="C16">
-        <v>-1.99</v>
+        <v>1.49</v>
       </c>
       <c r="D16">
-        <v>-0.41</v>
+        <v>0.04</v>
       </c>
       <c r="E16">
-        <v>11.86</v>
+        <v>8.59</v>
       </c>
       <c r="F16">
-        <v>-19.26</v>
+        <v>-17.93</v>
       </c>
       <c r="G16">
-        <v>3.37</v>
+        <v>-3.62</v>
       </c>
       <c r="H16">
-        <v>15.68</v>
+        <v>17.41</v>
       </c>
       <c r="I16">
-        <v>11.35</v>
+        <v>12.35</v>
       </c>
       <c r="J16">
-        <v>59.76</v>
+        <v>58.62</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1026,28 +1026,28 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>124.45</v>
+        <v>120.58</v>
       </c>
       <c r="C17">
-        <v>-0.52</v>
+        <v>-3.11</v>
       </c>
       <c r="D17">
-        <v>1.58</v>
+        <v>-2.17</v>
       </c>
       <c r="E17">
-        <v>12.6</v>
+        <v>6.93</v>
       </c>
       <c r="F17">
-        <v>17.96</v>
+        <v>16.03</v>
       </c>
       <c r="G17">
-        <v>40.72</v>
+        <v>38.44</v>
       </c>
       <c r="H17">
-        <v>46.12</v>
+        <v>41.58</v>
       </c>
       <c r="I17">
-        <v>32.86</v>
+        <v>29.25</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1055,31 +1055,31 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>310.95</v>
+        <v>310.76</v>
       </c>
       <c r="C18">
-        <v>-1.28</v>
+        <v>-0.06</v>
       </c>
       <c r="D18">
-        <v>-0.28</v>
+        <v>-1.6</v>
       </c>
       <c r="E18">
-        <v>20.07</v>
+        <v>20.22</v>
       </c>
       <c r="F18">
-        <v>-2.4</v>
+        <v>-0.61</v>
       </c>
       <c r="G18">
-        <v>0.13</v>
+        <v>-0.45</v>
       </c>
       <c r="H18">
-        <v>17.18</v>
+        <v>17.11</v>
       </c>
       <c r="I18">
-        <v>18.39</v>
+        <v>20.08</v>
       </c>
       <c r="J18">
-        <v>79.06</v>
+        <v>75.61</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1087,31 +1087,31 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>2039.7</v>
+        <v>2047.1</v>
       </c>
       <c r="C19">
-        <v>1.39</v>
+        <v>0.36</v>
       </c>
       <c r="D19">
-        <v>2.02</v>
+        <v>2.8</v>
       </c>
       <c r="E19">
-        <v>2.57</v>
+        <v>2.55</v>
       </c>
       <c r="F19">
-        <v>4.91</v>
+        <v>5.62</v>
       </c>
       <c r="G19">
-        <v>3.12</v>
+        <v>4.85</v>
       </c>
       <c r="H19">
-        <v>12.09</v>
+        <v>12.5</v>
       </c>
       <c r="I19">
-        <v>17.22</v>
+        <v>17.08</v>
       </c>
       <c r="J19">
-        <v>66.63</v>
+        <v>67.77</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1119,31 +1119,31 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>24.93</v>
+        <v>25.07</v>
       </c>
       <c r="C20">
-        <v>1.05</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D20">
-        <v>4.57</v>
+        <v>5.91</v>
       </c>
       <c r="E20">
-        <v>9.49</v>
+        <v>7.69</v>
       </c>
       <c r="F20">
-        <v>0.8100000000000001</v>
+        <v>2.45</v>
       </c>
       <c r="G20">
-        <v>4.4</v>
+        <v>6.05</v>
       </c>
       <c r="H20">
-        <v>4.48</v>
+        <v>5.07</v>
       </c>
       <c r="I20">
-        <v>19.23</v>
+        <v>18.25</v>
       </c>
       <c r="J20">
-        <v>74.7</v>
+        <v>77.93000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1151,31 +1151,31 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>944.1</v>
+        <v>936.4</v>
       </c>
       <c r="C21">
-        <v>2.94</v>
+        <v>-0.82</v>
       </c>
       <c r="D21">
-        <v>0.44</v>
+        <v>1.28</v>
       </c>
       <c r="E21">
-        <v>5.23</v>
+        <v>0.49</v>
       </c>
       <c r="F21">
-        <v>-3.68</v>
+        <v>-3.59</v>
       </c>
       <c r="G21">
-        <v>-7.28</v>
+        <v>-7.43</v>
       </c>
       <c r="H21">
-        <v>-12.07</v>
+        <v>-12.79</v>
       </c>
       <c r="I21">
-        <v>-7.17</v>
+        <v>-8.34</v>
       </c>
       <c r="J21">
-        <v>15.26</v>
+        <v>17.34</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1183,31 +1183,31 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <v>1057.4</v>
+        <v>1026.6</v>
       </c>
       <c r="C22">
-        <v>-0.29</v>
+        <v>-2.91</v>
       </c>
       <c r="D22">
-        <v>-3.27</v>
+        <v>-2.62</v>
       </c>
       <c r="E22">
-        <v>-5.94</v>
+        <v>-9.5</v>
       </c>
       <c r="F22">
-        <v>-13.11</v>
+        <v>-15</v>
       </c>
       <c r="G22">
-        <v>-23.15</v>
+        <v>-25.97</v>
       </c>
       <c r="H22">
-        <v>-40.9</v>
+        <v>-42.63</v>
       </c>
       <c r="I22">
-        <v>-42.36</v>
+        <v>-43.48</v>
       </c>
       <c r="J22">
-        <v>-9.109999999999999</v>
+        <v>-12.15</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1215,31 +1215,31 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>3.8</v>
+        <v>3.79</v>
       </c>
       <c r="C23">
-        <v>1.06</v>
+        <v>-0.26</v>
       </c>
       <c r="D23">
-        <v>-0.26</v>
+        <v>0.53</v>
       </c>
       <c r="E23">
-        <v>4.68</v>
+        <v>3.84</v>
       </c>
       <c r="F23">
-        <v>0.26</v>
+        <v>0.53</v>
       </c>
       <c r="G23">
-        <v>2.43</v>
+        <v>1.88</v>
       </c>
       <c r="H23">
-        <v>-0.26</v>
+        <v>-0.52</v>
       </c>
       <c r="I23">
-        <v>5.26</v>
+        <v>4.41</v>
       </c>
       <c r="J23">
-        <v>36.69</v>
+        <v>36.33</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1247,31 +1247,31 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>76.41</v>
+        <v>77.86</v>
       </c>
       <c r="C24">
-        <v>2.07</v>
+        <v>1.9</v>
       </c>
       <c r="D24">
-        <v>-1.75</v>
+        <v>0.99</v>
       </c>
       <c r="E24">
-        <v>-10.67</v>
+        <v>-5.41</v>
       </c>
       <c r="F24">
-        <v>-6.39</v>
+        <v>-6.9</v>
       </c>
       <c r="G24">
-        <v>9</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="H24">
-        <v>-4.8</v>
+        <v>-2.99</v>
       </c>
       <c r="I24">
-        <v>-1.07</v>
+        <v>-0.43</v>
       </c>
       <c r="J24">
-        <v>48.51</v>
+        <v>52.88</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1279,31 +1279,31 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>2039.7</v>
+        <v>2047.1</v>
       </c>
       <c r="C25">
-        <v>1.39</v>
+        <v>0.36</v>
       </c>
       <c r="D25">
-        <v>2.02</v>
+        <v>2.8</v>
       </c>
       <c r="E25">
-        <v>2.57</v>
+        <v>2.55</v>
       </c>
       <c r="F25">
-        <v>4.91</v>
+        <v>5.62</v>
       </c>
       <c r="G25">
-        <v>3.12</v>
+        <v>4.85</v>
       </c>
       <c r="H25">
-        <v>12.09</v>
+        <v>12.5</v>
       </c>
       <c r="I25">
-        <v>17.22</v>
+        <v>17.08</v>
       </c>
       <c r="J25">
-        <v>66.63</v>
+        <v>67.77</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1311,31 +1311,31 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <v>2.71</v>
+        <v>2.8</v>
       </c>
       <c r="C26">
-        <v>-2.87</v>
+        <v>3.32</v>
       </c>
       <c r="D26">
-        <v>-4.91</v>
+        <v>-3.45</v>
       </c>
       <c r="E26">
-        <v>-14.24</v>
+        <v>-16.42</v>
       </c>
       <c r="F26">
-        <v>-3.21</v>
+        <v>1.08</v>
       </c>
       <c r="G26">
-        <v>25.46</v>
+        <v>29.03</v>
       </c>
       <c r="H26">
-        <v>-39.37</v>
+        <v>-37.36</v>
       </c>
       <c r="I26">
-        <v>-59.61</v>
+        <v>-61.33</v>
       </c>
       <c r="J26">
-        <v>-41.72</v>
+        <v>-39.26</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1343,28 +1343,28 @@
         <v>34</v>
       </c>
       <c r="B27">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D27">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E27">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F27">
+        <v>0.03</v>
+      </c>
+      <c r="G27">
         <v>0.02</v>
-      </c>
-      <c r="G27">
-        <v>0.01</v>
       </c>
       <c r="H27">
         <v>-0.02</v>
       </c>
       <c r="I27">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <v>-0.09</v>
@@ -1375,7 +1375,7 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1390,7 +1390,7 @@
         <v>-0</v>
       </c>
       <c r="G28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>-0</v>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E29">
         <v>0.04</v>
@@ -1422,7 +1422,7 @@
         <v>0.01</v>
       </c>
       <c r="G29">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="H29">
         <v>0.03</v>
@@ -1431,7 +1431,7 @@
         <v>0.06</v>
       </c>
       <c r="J29">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1445,13 +1445,13 @@
         <v>0.01</v>
       </c>
       <c r="D30">
-        <v>-0</v>
+        <v>0.01</v>
       </c>
       <c r="E30">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F30">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="G30">
         <v>-0.05</v>
@@ -1463,7 +1463,7 @@
         <v>-0.06</v>
       </c>
       <c r="J30">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1474,28 +1474,28 @@
         <v>0.61</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D31">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E31">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F31">
+        <v>0.03</v>
+      </c>
+      <c r="G31">
         <v>0.02</v>
       </c>
-      <c r="G31">
-        <v>0.01</v>
-      </c>
       <c r="H31">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
       <c r="I31">
-        <v>-0.02</v>
+        <v>-0</v>
       </c>
       <c r="J31">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1506,10 +1506,10 @@
         <v>0.09</v>
       </c>
       <c r="C32">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0.05</v>
@@ -1524,7 +1524,7 @@
         <v>-0.07000000000000001</v>
       </c>
       <c r="I32">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
       <c r="J32">
         <v>-0.2</v>
@@ -1535,19 +1535,19 @@
         <v>40</v>
       </c>
       <c r="B33">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D33">
         <v>0.01</v>
       </c>
       <c r="E33">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F33">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>0.02</v>
@@ -1556,7 +1556,7 @@
         <v>0.05</v>
       </c>
       <c r="I33">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="J33">
         <v>-0.01</v>
@@ -1570,28 +1570,28 @@
         <v>0.1</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E34">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="F34">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="G34">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="J34">
-        <v>-0.13</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1605,13 +1605,13 @@
         <v>0</v>
       </c>
       <c r="D35">
+        <v>0.01</v>
+      </c>
+      <c r="E35">
+        <v>0.03</v>
+      </c>
+      <c r="F35">
         <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0.02</v>
-      </c>
-      <c r="F35">
-        <v>-0</v>
       </c>
       <c r="G35">
         <v>0.03</v>
@@ -1623,7 +1623,7 @@
         <v>0.08</v>
       </c>
       <c r="J35">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tips and cad fixed income
</commit_message>
<xml_diff>
--- a/finmail/output.xlsx
+++ b/finmail/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Price</t>
   </si>
@@ -58,18 +58,6 @@
     <t>CBOE Volatility Index</t>
   </si>
   <si>
-    <t>13 Week</t>
-  </si>
-  <si>
-    <t>5 Year</t>
-  </si>
-  <si>
-    <t>10 Year</t>
-  </si>
-  <si>
-    <t>30 Year</t>
-  </si>
-  <si>
     <t>Hudbay Minerals Inc.</t>
   </si>
   <si>
@@ -143,6 +131,33 @@
   </si>
   <si>
     <t>Swiss Franc</t>
+  </si>
+  <si>
+    <t>3 Month Treasury Yield</t>
+  </si>
+  <si>
+    <t>5 Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>10 Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>30 Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>1-3 Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>2 Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>5 Year TIPS Yield</t>
+  </si>
+  <si>
+    <t>10 Year TIPS Yield</t>
+  </si>
+  <si>
+    <t>30 Year TIPS Yield</t>
   </si>
 </sst>
 </file>
@@ -500,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -546,31 +561,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>454.61</v>
+        <v>472.7</v>
       </c>
       <c r="C2">
-        <v>-0.07000000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="D2">
-        <v>-0.09</v>
+        <v>0.55</v>
       </c>
       <c r="E2">
-        <v>9.390000000000001</v>
+        <v>4.71</v>
       </c>
       <c r="F2">
-        <v>1.3</v>
+        <v>10.27</v>
       </c>
       <c r="G2">
-        <v>7.01</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="H2">
-        <v>20.19</v>
+        <v>25.48</v>
       </c>
       <c r="I2">
-        <v>16.84</v>
+        <v>24.25</v>
       </c>
       <c r="J2">
-        <v>79.28</v>
+        <v>113.1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -578,31 +593,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>14258.49</v>
+        <v>14963.87</v>
       </c>
       <c r="C3">
-        <v>-0.16</v>
+        <v>1.26</v>
       </c>
       <c r="D3">
-        <v>-0.05</v>
+        <v>1.37</v>
       </c>
       <c r="E3">
-        <v>11.49</v>
+        <v>5.38</v>
       </c>
       <c r="F3">
-        <v>1.59</v>
+        <v>13.26</v>
       </c>
       <c r="G3">
-        <v>7.69</v>
+        <v>10.9</v>
       </c>
       <c r="H3">
-        <v>36.23</v>
+        <v>42.97</v>
       </c>
       <c r="I3">
-        <v>29.81</v>
+        <v>39.73</v>
       </c>
       <c r="J3">
-        <v>94.51000000000001</v>
+        <v>136.28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -610,31 +625,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>35430.42</v>
+        <v>37404.35</v>
       </c>
       <c r="C4">
-        <v>0.04</v>
+        <v>0.87</v>
       </c>
       <c r="D4">
-        <v>0.45</v>
+        <v>0.42</v>
       </c>
       <c r="E4">
-        <v>7.6</v>
+        <v>6.6</v>
       </c>
       <c r="F4">
-        <v>2.04</v>
+        <v>10.13</v>
       </c>
       <c r="G4">
-        <v>4.94</v>
+        <v>10.9</v>
       </c>
       <c r="H4">
-        <v>6.89</v>
+        <v>12.84</v>
       </c>
       <c r="I4">
-        <v>4.66</v>
+        <v>12.07</v>
       </c>
       <c r="J4">
-        <v>38.73</v>
+        <v>66.65000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -642,31 +657,31 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>12.98</v>
+        <v>13.65</v>
       </c>
       <c r="C5">
-        <v>2.29</v>
+        <v>-0.15</v>
       </c>
       <c r="D5">
-        <v>1.01</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="E5">
-        <v>-34.28</v>
+        <v>2.25</v>
       </c>
       <c r="F5">
-        <v>-4.35</v>
+        <v>-20.64</v>
       </c>
       <c r="G5">
-        <v>-11.1</v>
+        <v>1.56</v>
       </c>
       <c r="H5">
-        <v>-40.1</v>
+        <v>-37.01</v>
       </c>
       <c r="I5">
-        <v>-40.7</v>
+        <v>-31.99</v>
       </c>
       <c r="J5">
-        <v>-28.17</v>
+        <v>-54.67</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -674,31 +689,31 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>5.24</v>
+        <v>5.58</v>
       </c>
       <c r="C6">
-        <v>-0.38</v>
+        <v>2.39</v>
       </c>
       <c r="D6">
-        <v>-0.38</v>
+        <v>3.53</v>
       </c>
       <c r="E6">
-        <v>-1.32</v>
+        <v>22.64</v>
       </c>
       <c r="F6">
-        <v>-1.13</v>
+        <v>18.98</v>
       </c>
       <c r="G6">
-        <v>0.38</v>
+        <v>20.26</v>
       </c>
       <c r="H6">
-        <v>23</v>
+        <v>10.28</v>
       </c>
       <c r="I6">
-        <v>23.29</v>
+        <v>6.9</v>
       </c>
       <c r="J6">
-        <v>126.84</v>
+        <v>27.98</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -706,31 +721,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>4.22</v>
+        <v>125.17</v>
       </c>
       <c r="C7">
-        <v>-1.63</v>
+        <v>1.03</v>
       </c>
       <c r="D7">
-        <v>-4.95</v>
+        <v>4.32</v>
       </c>
       <c r="E7">
-        <v>-12.08</v>
+        <v>5.48</v>
       </c>
       <c r="F7">
-        <v>-0.47</v>
+        <v>11.11</v>
       </c>
       <c r="G7">
-        <v>9.9</v>
+        <v>8.33</v>
       </c>
       <c r="H7">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I7">
-        <v>7.65</v>
+        <v>3.6</v>
       </c>
       <c r="J7">
-        <v>48.07</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -738,31 +753,31 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>4.27</v>
+        <v>91.8</v>
       </c>
       <c r="C8">
-        <v>-1.61</v>
+        <v>0.14</v>
       </c>
       <c r="D8">
-        <v>-3.39</v>
+        <v>-1.43</v>
       </c>
       <c r="E8">
-        <v>-12.5</v>
+        <v>4.37</v>
       </c>
       <c r="F8">
-        <v>4.4</v>
+        <v>1.59</v>
       </c>
       <c r="G8">
-        <v>15.72</v>
+        <v>27.06</v>
       </c>
       <c r="H8">
-        <v>10.05</v>
+        <v>47.21</v>
       </c>
       <c r="I8">
-        <v>13.87</v>
+        <v>45.51</v>
       </c>
       <c r="J8">
-        <v>41.86</v>
+        <v>369.81</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -770,31 +785,31 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>4.45</v>
+        <v>423.44</v>
       </c>
       <c r="C9">
-        <v>-1.55</v>
+        <v>0.95</v>
       </c>
       <c r="D9">
-        <v>-2.2</v>
+        <v>1.17</v>
       </c>
       <c r="E9">
-        <v>-11.53</v>
+        <v>3.54</v>
       </c>
       <c r="F9">
-        <v>5.95</v>
+        <v>5.43</v>
       </c>
       <c r="G9">
-        <v>14.69</v>
+        <v>11.81</v>
       </c>
       <c r="H9">
-        <v>12.09</v>
+        <v>22.52</v>
       </c>
       <c r="I9">
-        <v>17.11</v>
+        <v>23.24</v>
       </c>
       <c r="J9">
-        <v>34.44</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -802,31 +817,31 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>4.48</v>
+        <v>194.68</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>-0.08</v>
       </c>
       <c r="D10">
-        <v>-0.44</v>
+        <v>-1.73</v>
       </c>
       <c r="E10">
-        <v>3.46</v>
+        <v>2.12</v>
       </c>
       <c r="F10">
-        <v>-9.859999999999999</v>
+        <v>11.53</v>
       </c>
       <c r="G10">
-        <v>-5.88</v>
+        <v>4.57</v>
       </c>
       <c r="H10">
-        <v>-11.46</v>
+        <v>50.67</v>
       </c>
       <c r="I10">
-        <v>-17.95</v>
+        <v>44.53</v>
       </c>
       <c r="J10">
-        <v>-10.4</v>
+        <v>438.24</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -834,31 +849,31 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>120.46</v>
+        <v>137.88</v>
       </c>
       <c r="C11">
-        <v>0.32</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="D11">
-        <v>-1.54</v>
+        <v>-2.11</v>
       </c>
       <c r="E11">
-        <v>6.32</v>
+        <v>1.48</v>
       </c>
       <c r="F11">
-        <v>3.06</v>
+        <v>16.02</v>
       </c>
       <c r="G11">
-        <v>2.44</v>
+        <v>10.41</v>
       </c>
       <c r="H11">
-        <v>1.75</v>
+        <v>13.55</v>
       </c>
       <c r="I11">
-        <v>0.79</v>
+        <v>13.25</v>
       </c>
       <c r="J11">
-        <v>113.73</v>
+        <v>83.38</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -866,31 +881,31 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>92.27</v>
+        <v>57.88</v>
       </c>
       <c r="C12">
-        <v>1.81</v>
+        <v>0.87</v>
       </c>
       <c r="D12">
-        <v>2.29</v>
+        <v>-0.87</v>
       </c>
       <c r="E12">
-        <v>15.68</v>
+        <v>18.03</v>
       </c>
       <c r="F12">
-        <v>6.17</v>
+        <v>2.14</v>
       </c>
       <c r="G12">
-        <v>33.76</v>
+        <v>4.42</v>
       </c>
       <c r="H12">
-        <v>47.96</v>
+        <v>37.09</v>
       </c>
       <c r="I12">
-        <v>43.34</v>
+        <v>34.2</v>
       </c>
       <c r="J12">
-        <v>297.89</v>
+        <v>130.14</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -898,31 +913,28 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>409.82</v>
+        <v>118.31</v>
       </c>
       <c r="C13">
-        <v>0.2</v>
+        <v>1.11</v>
       </c>
       <c r="D13">
-        <v>-0.12</v>
+        <v>2.34</v>
       </c>
       <c r="E13">
-        <v>10.04</v>
+        <v>-3.43</v>
       </c>
       <c r="F13">
-        <v>-0.54</v>
+        <v>7.46</v>
       </c>
       <c r="G13">
-        <v>9.970000000000001</v>
+        <v>31.59</v>
       </c>
       <c r="H13">
-        <v>18.58</v>
+        <v>38.91</v>
       </c>
       <c r="I13">
-        <v>20.16</v>
-      </c>
-      <c r="J13">
-        <v>109.55</v>
+        <v>33.58</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -930,31 +942,31 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>189.37</v>
+        <v>333.45</v>
       </c>
       <c r="C14">
-        <v>-0.54</v>
+        <v>2.46</v>
       </c>
       <c r="D14">
-        <v>-1.01</v>
+        <v>2.23</v>
       </c>
       <c r="E14">
-        <v>11.35</v>
+        <v>6.94</v>
       </c>
       <c r="F14">
-        <v>0.93</v>
+        <v>15.7</v>
       </c>
       <c r="G14">
-        <v>4.93</v>
+        <v>1.89</v>
       </c>
       <c r="H14">
-        <v>46.56</v>
+        <v>25.66</v>
       </c>
       <c r="I14">
-        <v>34.89</v>
+        <v>25.28</v>
       </c>
       <c r="J14">
-        <v>341.94</v>
+        <v>124.29</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -962,31 +974,31 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>137.31</v>
+        <v>2039.1</v>
       </c>
       <c r="C15">
-        <v>0.68</v>
+        <v>0.23</v>
       </c>
       <c r="D15">
-        <v>1.02</v>
+        <v>0.44</v>
       </c>
       <c r="E15">
-        <v>13.35</v>
+        <v>1.99</v>
       </c>
       <c r="F15">
-        <v>14.61</v>
+        <v>5.91</v>
       </c>
       <c r="G15">
-        <v>7.87</v>
+        <v>6.25</v>
       </c>
       <c r="H15">
-        <v>13.08</v>
+        <v>12.06</v>
       </c>
       <c r="I15">
-        <v>8.289999999999999</v>
+        <v>12.29</v>
       </c>
       <c r="J15">
-        <v>66.31999999999999</v>
+        <v>62.63</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -994,31 +1006,31 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>49.57</v>
+        <v>24.31</v>
       </c>
       <c r="C16">
-        <v>1.49</v>
+        <v>-0.16</v>
       </c>
       <c r="D16">
-        <v>0.04</v>
+        <v>0.87</v>
       </c>
       <c r="E16">
-        <v>8.59</v>
+        <v>1.97</v>
       </c>
       <c r="F16">
-        <v>-17.93</v>
+        <v>3.01</v>
       </c>
       <c r="G16">
-        <v>-3.62</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="H16">
-        <v>17.41</v>
+        <v>1.89</v>
       </c>
       <c r="I16">
-        <v>12.35</v>
+        <v>1.17</v>
       </c>
       <c r="J16">
-        <v>58.62</v>
+        <v>66.73999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1026,28 +1038,31 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>120.58</v>
+        <v>967.6</v>
       </c>
       <c r="C17">
-        <v>-3.11</v>
+        <v>-0.38</v>
       </c>
       <c r="D17">
-        <v>-2.17</v>
+        <v>0.26</v>
       </c>
       <c r="E17">
-        <v>6.93</v>
+        <v>2.94</v>
       </c>
       <c r="F17">
-        <v>16.03</v>
+        <v>3.59</v>
       </c>
       <c r="G17">
-        <v>38.44</v>
+        <v>3.84</v>
       </c>
       <c r="H17">
-        <v>41.58</v>
+        <v>-9.880000000000001</v>
       </c>
       <c r="I17">
-        <v>29.25</v>
+        <v>-4.67</v>
+      </c>
+      <c r="J17">
+        <v>21.77</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1055,31 +1070,31 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>310.76</v>
+        <v>1216.7</v>
       </c>
       <c r="C18">
-        <v>-0.06</v>
+        <v>0.11</v>
       </c>
       <c r="D18">
-        <v>-1.6</v>
+        <v>9.44</v>
       </c>
       <c r="E18">
-        <v>20.22</v>
+        <v>11.31</v>
       </c>
       <c r="F18">
-        <v>-0.61</v>
+        <v>-2.29</v>
       </c>
       <c r="G18">
-        <v>-0.45</v>
+        <v>-4.05</v>
       </c>
       <c r="H18">
-        <v>17.11</v>
+        <v>-32</v>
       </c>
       <c r="I18">
-        <v>20.08</v>
+        <v>-26.01</v>
       </c>
       <c r="J18">
-        <v>75.61</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1087,31 +1102,31 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>2047.1</v>
+        <v>3.91</v>
       </c>
       <c r="C19">
-        <v>0.36</v>
+        <v>0.26</v>
       </c>
       <c r="D19">
-        <v>2.8</v>
+        <v>0.51</v>
       </c>
       <c r="E19">
-        <v>2.55</v>
+        <v>2.62</v>
       </c>
       <c r="F19">
-        <v>5.62</v>
+        <v>6.54</v>
       </c>
       <c r="G19">
-        <v>4.85</v>
+        <v>2.62</v>
       </c>
       <c r="H19">
-        <v>12.5</v>
+        <v>2.62</v>
       </c>
       <c r="I19">
-        <v>17.08</v>
+        <v>2.62</v>
       </c>
       <c r="J19">
-        <v>67.77</v>
+        <v>45.9</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1119,191 +1134,191 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>25.07</v>
+        <v>73.89</v>
       </c>
       <c r="C20">
-        <v>0.5600000000000001</v>
+        <v>-0.44</v>
       </c>
       <c r="D20">
-        <v>5.91</v>
+        <v>3.23</v>
       </c>
       <c r="E20">
-        <v>7.69</v>
+        <v>-4.99</v>
       </c>
       <c r="F20">
-        <v>2.45</v>
+        <v>-17.93</v>
       </c>
       <c r="G20">
-        <v>6.05</v>
+        <v>6.84</v>
       </c>
       <c r="H20">
-        <v>5.07</v>
+        <v>-7.94</v>
       </c>
       <c r="I20">
-        <v>18.25</v>
+        <v>-5.62</v>
       </c>
       <c r="J20">
-        <v>77.93000000000001</v>
+        <v>62.08</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B21">
-        <v>936.4</v>
+        <v>2039.1</v>
       </c>
       <c r="C21">
-        <v>-0.82</v>
+        <v>0.23</v>
       </c>
       <c r="D21">
-        <v>1.28</v>
+        <v>0.44</v>
       </c>
       <c r="E21">
-        <v>0.49</v>
+        <v>1.99</v>
       </c>
       <c r="F21">
-        <v>-3.59</v>
+        <v>5.91</v>
       </c>
       <c r="G21">
-        <v>-7.43</v>
+        <v>6.25</v>
       </c>
       <c r="H21">
-        <v>-12.79</v>
+        <v>12.06</v>
       </c>
       <c r="I21">
-        <v>-8.34</v>
+        <v>12.29</v>
       </c>
       <c r="J21">
-        <v>17.34</v>
+        <v>62.63</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>1026.6</v>
+        <v>2.57</v>
       </c>
       <c r="C22">
-        <v>-2.91</v>
+        <v>4.9</v>
       </c>
       <c r="D22">
-        <v>-2.62</v>
+        <v>7.53</v>
       </c>
       <c r="E22">
-        <v>-9.5</v>
+        <v>-9.82</v>
       </c>
       <c r="F22">
-        <v>-15</v>
+        <v>-2.65</v>
       </c>
       <c r="G22">
-        <v>-25.97</v>
+        <v>-5.86</v>
       </c>
       <c r="H22">
-        <v>-42.63</v>
+        <v>-42.51</v>
       </c>
       <c r="I22">
-        <v>-43.48</v>
+        <v>-51.78</v>
       </c>
       <c r="J22">
-        <v>-12.15</v>
+        <v>-32.72</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>3.79</v>
+        <v>0.67</v>
       </c>
       <c r="C23">
-        <v>-0.26</v>
+        <v>-0</v>
       </c>
       <c r="D23">
-        <v>0.53</v>
+        <v>0.01</v>
       </c>
       <c r="E23">
-        <v>3.84</v>
+        <v>0.03</v>
       </c>
       <c r="F23">
-        <v>0.53</v>
+        <v>0.05</v>
       </c>
       <c r="G23">
-        <v>1.88</v>
+        <v>-0.01</v>
       </c>
       <c r="H23">
-        <v>-0.52</v>
+        <v>-0</v>
       </c>
       <c r="I23">
-        <v>4.41</v>
+        <v>0.01</v>
       </c>
       <c r="J23">
-        <v>36.33</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>77.86</v>
+        <v>0.75</v>
       </c>
       <c r="C24">
-        <v>1.9</v>
+        <v>-0</v>
       </c>
       <c r="D24">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
       <c r="E24">
-        <v>-5.41</v>
+        <v>0.03</v>
       </c>
       <c r="F24">
-        <v>-6.9</v>
+        <v>0.01</v>
       </c>
       <c r="G24">
-        <v>8.529999999999999</v>
+        <v>-0.01</v>
       </c>
       <c r="H24">
-        <v>-2.99</v>
+        <v>0.01</v>
       </c>
       <c r="I24">
-        <v>-0.43</v>
+        <v>0.02</v>
       </c>
       <c r="J24">
-        <v>52.88</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>2047.1</v>
+        <v>1.09</v>
       </c>
       <c r="C25">
-        <v>0.36</v>
+        <v>-0</v>
       </c>
       <c r="D25">
-        <v>2.8</v>
+        <v>0.01</v>
       </c>
       <c r="E25">
-        <v>2.55</v>
+        <v>-0</v>
       </c>
       <c r="F25">
-        <v>5.62</v>
+        <v>0.03</v>
       </c>
       <c r="G25">
-        <v>4.85</v>
+        <v>-0</v>
       </c>
       <c r="H25">
-        <v>12.5</v>
+        <v>0.03</v>
       </c>
       <c r="I25">
-        <v>17.08</v>
+        <v>0.03</v>
       </c>
       <c r="J25">
-        <v>67.77</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1311,31 +1326,31 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <v>2.8</v>
+        <v>0.01</v>
       </c>
       <c r="C26">
-        <v>3.32</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>-3.45</v>
+        <v>-0.01</v>
       </c>
       <c r="E26">
-        <v>-16.42</v>
+        <v>0.03</v>
       </c>
       <c r="F26">
-        <v>1.08</v>
+        <v>0.03</v>
       </c>
       <c r="G26">
-        <v>29.03</v>
+        <v>-0.01</v>
       </c>
       <c r="H26">
-        <v>-37.36</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="I26">
-        <v>-61.33</v>
+        <v>-0.08</v>
       </c>
       <c r="J26">
-        <v>-39.26</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1343,31 +1358,31 @@
         <v>34</v>
       </c>
       <c r="B27">
-        <v>0.67</v>
+        <v>0.63</v>
       </c>
       <c r="C27">
+        <v>-0</v>
+      </c>
+      <c r="D27">
         <v>0.01</v>
       </c>
-      <c r="D27">
-        <v>0.02</v>
-      </c>
       <c r="E27">
+        <v>0.04</v>
+      </c>
+      <c r="F27">
         <v>0.05</v>
       </c>
-      <c r="F27">
-        <v>0.03</v>
-      </c>
       <c r="G27">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H27">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="J27">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1375,31 +1390,31 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>0.74</v>
+        <v>0.1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="D28">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E28">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F28">
-        <v>-0</v>
+        <v>0.04</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H28">
-        <v>-0</v>
+        <v>-0.04</v>
       </c>
       <c r="I28">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="J28">
-        <v>-0.02</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1407,31 +1422,31 @@
         <v>36</v>
       </c>
       <c r="B29">
-        <v>1.1</v>
+        <v>1.26</v>
       </c>
       <c r="C29">
+        <v>-0.01</v>
+      </c>
+      <c r="D29">
         <v>0</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>0.01</v>
       </c>
-      <c r="E29">
+      <c r="F29">
+        <v>0.03</v>
+      </c>
+      <c r="G29">
+        <v>-0.01</v>
+      </c>
+      <c r="H29">
+        <v>0.05</v>
+      </c>
+      <c r="I29">
         <v>0.04</v>
       </c>
-      <c r="F29">
-        <v>0.01</v>
-      </c>
-      <c r="G29">
-        <v>0.03</v>
-      </c>
-      <c r="H29">
-        <v>0.03</v>
-      </c>
-      <c r="I29">
-        <v>0.06</v>
-      </c>
       <c r="J29">
-        <v>-0.03</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1439,31 +1454,31 @@
         <v>37</v>
       </c>
       <c r="B30">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C30">
-        <v>0.01</v>
+        <v>-0</v>
       </c>
       <c r="D30">
         <v>0.01</v>
       </c>
       <c r="E30">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F30">
-        <v>-0.01</v>
+        <v>0.1</v>
       </c>
       <c r="G30">
-        <v>-0.05</v>
+        <v>0.05</v>
       </c>
       <c r="H30">
-        <v>-0.1</v>
+        <v>0.03</v>
       </c>
       <c r="I30">
-        <v>-0.06</v>
+        <v>0.03</v>
       </c>
       <c r="J30">
-        <v>-0.23</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1471,31 +1486,31 @@
         <v>38</v>
       </c>
       <c r="B31">
-        <v>0.61</v>
+        <v>1.16</v>
       </c>
       <c r="C31">
+        <v>-0</v>
+      </c>
+      <c r="D31">
         <v>0.01</v>
       </c>
-      <c r="D31">
-        <v>0.02</v>
-      </c>
       <c r="E31">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F31">
+        <v>0.05</v>
+      </c>
+      <c r="G31">
         <v>0.03</v>
       </c>
-      <c r="G31">
-        <v>0.02</v>
-      </c>
       <c r="H31">
-        <v>-0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I31">
-        <v>-0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J31">
-        <v>-0.1</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1503,31 +1518,31 @@
         <v>39</v>
       </c>
       <c r="B32">
-        <v>0.09</v>
+        <v>5.21</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>-0.38</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>-0.19</v>
       </c>
       <c r="E32">
-        <v>0.05</v>
+        <v>-0.95</v>
       </c>
       <c r="F32">
-        <v>-0</v>
+        <v>-1.7</v>
       </c>
       <c r="G32">
-        <v>0.05</v>
+        <v>1.36</v>
       </c>
       <c r="H32">
-        <v>-0.07000000000000001</v>
+        <v>22.3</v>
       </c>
       <c r="I32">
-        <v>-0.06</v>
+        <v>24.05</v>
       </c>
       <c r="J32">
-        <v>-0.2</v>
+        <v>123.61</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1535,31 +1550,31 @@
         <v>40</v>
       </c>
       <c r="B33">
-        <v>1.27</v>
+        <v>3.88</v>
       </c>
       <c r="C33">
-        <v>0.01</v>
+        <v>0.26</v>
       </c>
       <c r="D33">
-        <v>0.01</v>
+        <v>-0.77</v>
       </c>
       <c r="E33">
-        <v>0.05</v>
+        <v>-12.22</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>-15.1</v>
       </c>
       <c r="G33">
-        <v>0.02</v>
+        <v>-2.76</v>
       </c>
       <c r="H33">
-        <v>0.05</v>
+        <v>-3</v>
       </c>
       <c r="I33">
-        <v>0.06</v>
+        <v>2.65</v>
       </c>
       <c r="J33">
-        <v>-0.01</v>
+        <v>46.97</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1567,31 +1582,31 @@
         <v>41</v>
       </c>
       <c r="B34">
-        <v>0.1</v>
+        <v>3.89</v>
       </c>
       <c r="C34">
-        <v>0.01</v>
+        <v>0.26</v>
       </c>
       <c r="D34">
-        <v>0.01</v>
+        <v>-1.02</v>
       </c>
       <c r="E34">
-        <v>0.08</v>
+        <v>-11.99</v>
       </c>
       <c r="F34">
-        <v>0.05</v>
+        <v>-12.39</v>
       </c>
       <c r="G34">
-        <v>0.05</v>
+        <v>4.01</v>
       </c>
       <c r="H34">
-        <v>0.01</v>
+        <v>0.26</v>
       </c>
       <c r="I34">
-        <v>0.02</v>
+        <v>5.71</v>
       </c>
       <c r="J34">
-        <v>-0.12</v>
+        <v>39.43</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1599,31 +1614,255 @@
         <v>42</v>
       </c>
       <c r="B35">
-        <v>1.14</v>
+        <v>4.04</v>
       </c>
       <c r="C35">
+        <v>0.75</v>
+      </c>
+      <c r="D35">
+        <v>-0.25</v>
+      </c>
+      <c r="E35">
+        <v>-11.79</v>
+      </c>
+      <c r="F35">
+        <v>-10.62</v>
+      </c>
+      <c r="G35">
+        <v>5.76</v>
+      </c>
+      <c r="H35">
+        <v>1.76</v>
+      </c>
+      <c r="I35">
+        <v>8.02</v>
+      </c>
+      <c r="J35">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>3.94</v>
+      </c>
+      <c r="C36">
         <v>0</v>
       </c>
-      <c r="D35">
-        <v>0.01</v>
-      </c>
-      <c r="E35">
-        <v>0.03</v>
-      </c>
-      <c r="F35">
+      <c r="D36">
+        <v>0.51</v>
+      </c>
+      <c r="E36">
+        <v>11.93</v>
+      </c>
+      <c r="F36">
+        <v>23.86</v>
+      </c>
+      <c r="G36">
+        <v>17.01</v>
+      </c>
+      <c r="H36">
+        <v>3.3</v>
+      </c>
+      <c r="I36">
+        <v>-2.79</v>
+      </c>
+      <c r="J36">
+        <v>-51.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>3.91</v>
+      </c>
+      <c r="C37">
         <v>0</v>
       </c>
-      <c r="G35">
-        <v>0.03</v>
-      </c>
-      <c r="H35">
-        <v>0.05</v>
-      </c>
-      <c r="I35">
-        <v>0.08</v>
-      </c>
-      <c r="J35">
-        <v>0.14</v>
+      <c r="D37">
+        <v>0.77</v>
+      </c>
+      <c r="E37">
+        <v>12.53</v>
+      </c>
+      <c r="F37">
+        <v>25.83</v>
+      </c>
+      <c r="G37">
+        <v>19.18</v>
+      </c>
+      <c r="H37">
+        <v>3.84</v>
+      </c>
+      <c r="I37">
+        <v>-2.3</v>
+      </c>
+      <c r="J37">
+        <v>-50.38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>3.18</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1.89</v>
+      </c>
+      <c r="E38">
+        <v>18.24</v>
+      </c>
+      <c r="F38">
+        <v>32.39</v>
+      </c>
+      <c r="G38">
+        <v>18.24</v>
+      </c>
+      <c r="H38">
+        <v>7.23</v>
+      </c>
+      <c r="I38">
+        <v>-0.9399999999999999</v>
+      </c>
+      <c r="J38">
+        <v>-38.36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>3.06</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1.63</v>
+      </c>
+      <c r="E39">
+        <v>19.28</v>
+      </c>
+      <c r="F39">
+        <v>27.78</v>
+      </c>
+      <c r="G39">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="H39">
+        <v>7.84</v>
+      </c>
+      <c r="I39">
+        <v>0.65</v>
+      </c>
+      <c r="J39">
+        <v>-33.99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>2.18</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>-0.46</v>
+      </c>
+      <c r="E40">
+        <v>1.38</v>
+      </c>
+      <c r="F40">
+        <v>5.05</v>
+      </c>
+      <c r="G40">
+        <v>-0.92</v>
+      </c>
+      <c r="H40">
+        <v>6.88</v>
+      </c>
+      <c r="I40">
+        <v>2.75</v>
+      </c>
+      <c r="J40">
+        <v>-28.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>2.19</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1.37</v>
+      </c>
+      <c r="E41">
+        <v>3.2</v>
+      </c>
+      <c r="F41">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="G41">
+        <v>0.91</v>
+      </c>
+      <c r="H41">
+        <v>5.02</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>-19.18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <v>2.4</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>-2.5</v>
+      </c>
+      <c r="G42">
+        <v>-7.08</v>
+      </c>
+      <c r="H42">
+        <v>-6.67</v>
+      </c>
+      <c r="I42">
+        <v>-5.83</v>
+      </c>
+      <c r="J42">
+        <v>-20.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>